<commit_message>
All user services done
</commit_message>
<xml_diff>
--- a/practice/.net/unidad 4 webapi/unidad 4 webapi/BibliotecaBaseDatos.xlsx
+++ b/practice/.net/unidad 4 webapi/unidad 4 webapi/BibliotecaBaseDatos.xlsx
@@ -98,6 +98,18 @@
   </x:si>
   <x:si>
     <x:t>adel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>a borrar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2222</x:t>
+  </x:si>
+  <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
+    <x:t>solito despues de borrar</x:t>
   </x:si>
   <x:si>
     <x:t>Accion</x:t>
@@ -874,13 +886,55 @@
         <x:v>12313123</x:v>
       </x:c>
       <x:c r="B21" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="C21" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
       <x:c r="D21" s="0" t="s">
         <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="22" spans="1:4">
+      <x:c r="A22" s="0">
+        <x:v>12313124</x:v>
+      </x:c>
+      <x:c r="B22" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C22" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D22" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="23" spans="1:4">
+      <x:c r="A23" s="0">
+        <x:v>12313124</x:v>
+      </x:c>
+      <x:c r="B23" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="C23" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D23" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="24" spans="1:4">
+      <x:c r="A24" s="0">
+        <x:v>99999991</x:v>
+      </x:c>
+      <x:c r="B24" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="C24" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="D24" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
   </x:sheetData>
@@ -918,10 +972,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="E1" s="1"/>
     </x:row>
@@ -933,10 +987,10 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>30</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -947,7 +1001,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
         <x:v>6</x:v>
@@ -961,10 +1015,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,7 +1029,7 @@
         <x:v>7</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
         <x:v>9</x:v>
@@ -989,7 +1043,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
         <x:v>6</x:v>
@@ -1003,7 +1057,7 @@
         <x:v>12</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
         <x:v>6</x:v>
@@ -1017,7 +1071,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
         <x:v>9</x:v>
@@ -1028,10 +1082,10 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
         <x:v>9</x:v>
@@ -1045,7 +1099,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
         <x:v>9</x:v>
@@ -1059,7 +1113,7 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
         <x:v>9</x:v>
@@ -1073,7 +1127,7 @@
         <x:v>13</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
         <x:v>9</x:v>
@@ -1087,7 +1141,7 @@
         <x:v>19</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
         <x:v>6</x:v>
@@ -1101,7 +1155,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
         <x:v>9</x:v>
@@ -1115,7 +1169,7 @@
         <x:v>4</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
         <x:v>6</x:v>
@@ -1147,33 +1201,33 @@
   <x:sheetData>
     <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A1" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B1" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C1" s="1" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D1" s="1" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E1" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>39</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <x:c r="A2" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="E2" s="0">
         <x:v>10</x:v>
@@ -1187,10 +1241,10 @@
         <x:v>6</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E3" s="0">
         <x:v>11</x:v>
@@ -1201,13 +1255,13 @@
         <x:v>102</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E4" s="0">
         <x:v>12</x:v>
@@ -1221,10 +1275,10 @@
         <x:v>9</x:v>
       </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E5" s="0">
         <x:v>13</x:v>
@@ -1235,13 +1289,13 @@
         <x:v>104</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
         <x:v>41</x:v>
-      </x:c>
-      <x:c r="C6" s="0" t="s">
-        <x:v>36</x:v>
-      </x:c>
-      <x:c r="D6" s="0" t="s">
-        <x:v>37</x:v>
       </x:c>
       <x:c r="E6" s="0">
         <x:v>14</x:v>
@@ -1252,13 +1306,13 @@
         <x:v>105</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
         <x:v>42</x:v>
       </x:c>
-      <x:c r="C7" s="0" t="s">
-        <x:v>38</x:v>
-      </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E7" s="0">
         <x:v>15</x:v>
@@ -1269,13 +1323,13 @@
         <x:v>106</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
-      <x:c r="C8" s="0" t="s">
-        <x:v>39</x:v>
-      </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E8" s="0">
         <x:v>16</x:v>
@@ -1286,13 +1340,13 @@
         <x:v>107</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E9" s="0">
         <x:v>17</x:v>
@@ -1303,13 +1357,13 @@
         <x:v>108</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E10" s="0">
         <x:v>18</x:v>
@@ -1320,13 +1374,13 @@
         <x:v>109</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E11" s="0">
         <x:v>19</x:v>
@@ -1337,13 +1391,13 @@
         <x:v>110</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E12" s="0">
         <x:v>20</x:v>
@@ -1354,13 +1408,13 @@
         <x:v>111</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>52</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E13" s="0">
         <x:v>21</x:v>
@@ -1371,13 +1425,13 @@
         <x:v>112</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="E14" s="0">
         <x:v>22</x:v>
@@ -1388,13 +1442,13 @@
         <x:v>113</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>56</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>57</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="E15" s="0">
         <x:v>23</x:v>

</xml_diff>